<commit_message>
Atualização dos Documentos Organizacionais
</commit_message>
<xml_diff>
--- a/Documentos Organizacional/Plano de Ação .xlsx
+++ b/Documentos Organizacional/Plano de Ação .xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelvi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\EcoYield\Documentos Organizacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4613675-BC29-449F-9F77-010F8D2F425D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECFC959-EEDC-48F9-A7ED-5E964BA55829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8F06A637-B259-457E-B777-57329A3DB9A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F06A637-B259-457E-B777-57329A3DB9A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Tarefa</t>
   </si>
@@ -60,6 +60,54 @@
   </si>
   <si>
     <t xml:space="preserve">Plano de Ação - Projeto EcoYield </t>
+  </si>
+  <si>
+    <t>Fazendo</t>
+  </si>
+  <si>
+    <t>Entregar novo protótipo de Calculadora</t>
+  </si>
+  <si>
+    <t>Enrico e Samuel</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Modificações na documentação</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Novo Banco de Dados com DER</t>
+  </si>
+  <si>
+    <t>Modificações nos Slides de Apresentação</t>
+  </si>
+  <si>
+    <t>Larissa e Tabata</t>
+  </si>
+  <si>
+    <t>Protótipo do Site no Figma</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Kaue</t>
+  </si>
+  <si>
+    <t>Criação do Site por código</t>
+  </si>
+  <si>
+    <t>A Fazer</t>
+  </si>
+  <si>
+    <t>Verificação do código de arduino</t>
+  </si>
+  <si>
+    <t>Cristhian e Kaue</t>
   </si>
 </sst>
 </file>
@@ -120,12 +168,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -209,23 +264,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BF44E57-967C-419F-9AB8-BDCC3352680F}" name="Tabela1" displayName="Tabela1" ref="C6:I21" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BF44E57-967C-419F-9AB8-BDCC3352680F}" name="Tabela1" displayName="Tabela1" ref="C6:I21" dataDxfId="7">
   <autoFilter ref="C6:I21" xr:uid="{7BF44E57-967C-419F-9AB8-BDCC3352680F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7B3C59AA-ED28-46CE-8305-B8C794F7FB06}" name="Tarefa" totalsRowLabel="Total" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{F2329F20-75D5-48E7-B486-7F65B2514E6C}" name="Prioridade" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{91EE20C7-C9F9-4087-AFAD-2FD6F584CAD8}" name="Status" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{10B1D8CE-E5C1-4CCE-BD2D-444145E19FBB}" name="Prazo" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{C349E915-4FED-4B28-9BF0-54C673FFFD28}" name="Responsável" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{FBC9FCB6-613A-440E-AF29-44B3A5AF0EB9}" name="Concluido %" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{2F6AA06C-FC45-4B8D-8F1D-F0C733AA7E1C}" name="Anotações" totalsRowFunction="count" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7B3C59AA-ED28-46CE-8305-B8C794F7FB06}" name="Tarefa" totalsRowLabel="Total" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F2329F20-75D5-48E7-B486-7F65B2514E6C}" name="Prioridade" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{91EE20C7-C9F9-4087-AFAD-2FD6F584CAD8}" name="Status" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{10B1D8CE-E5C1-4CCE-BD2D-444145E19FBB}" name="Prazo" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{C349E915-4FED-4B28-9BF0-54C673FFFD28}" name="Responsável" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{FBC9FCB6-613A-440E-AF29-44B3A5AF0EB9}" name="Concluido %" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{2F6AA06C-FC45-4B8D-8F1D-F0C733AA7E1C}" name="Anotações" totalsRowFunction="count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -544,13 +599,13 @@
   <dimension ref="C3:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="114" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
@@ -571,21 +626,21 @@
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -611,64 +666,132 @@
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6">
+        <v>45394</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="7">
+        <v>45394</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6">
+        <v>45394</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="7">
+        <v>45394</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="6">
+        <v>45396</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="7">
+        <v>45394</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="6">
+        <v>45398</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -747,8 +870,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>